<commit_message>
Admon dashboard to excel
</commit_message>
<xml_diff>
--- a/app/templates/report/dashboard.pay.xlsx
+++ b/app/templates/report/dashboard.pay.xlsx
@@ -8,31 +8,94 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0563B611-0E4D-4C0F-84C0-209C9A523EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F307C79-D5C7-4E8A-AD9B-CC03165AAE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Payments" sheetId="1" r:id="rId1"/>
+    <sheet name="Pending payments" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+  <si>
+    <t>Id reserva</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>Fecha de fin</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Recurso</t>
+  </si>
+  <si>
+    <t>Fecha de emisión</t>
+  </si>
+  <si>
+    <t>Id
+Pago</t>
+  </si>
+  <si>
+    <t>Importe</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Facturas</t>
+  </si>
+  <si>
+    <t>Método de pago</t>
+  </si>
+  <si>
+    <t>Aviso 1</t>
+  </si>
+  <si>
+    <t>Aviso 2</t>
+  </si>
+  <si>
+    <t>Aviso 3</t>
+  </si>
+  <si>
+    <t>Pagos pendientes</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -63,13 +126,20 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -90,11 +160,10 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00BFB2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,10 +173,25 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC6C6C6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
       </right>
       <top/>
       <bottom/>
@@ -119,21 +203,41 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -519,28 +623,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.85546875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="24.85546875" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="44.140625" style="9" customWidth="1"/>
+    <col min="13" max="15" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="24.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>